<commit_message>
stok modeline tarih sutunu eklendi
</commit_message>
<xml_diff>
--- a/etikom/static/file/ornek-stok-dosyasi.xlsx
+++ b/etikom/static/file/ornek-stok-dosyasi.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29127"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD7A60A2-227A-4C96-8700-A7DB2BDEAC1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D92B19-2F8E-4515-B7F6-55D3EF63E3F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
   <si>
     <t>Fatura No</t>
   </si>
@@ -75,6 +75,9 @@
   </si>
   <si>
     <t>BELGENO00183346</t>
+  </si>
+  <si>
+    <t>Fatura Tarihi</t>
   </si>
 </sst>
 </file>
@@ -164,7 +167,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -199,6 +202,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -505,414 +515,467 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="21.578125" customWidth="1"/>
-    <col min="2" max="2" width="14.68359375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="10.5234375" customWidth="1"/>
-    <col min="4" max="4" width="12.05078125" customWidth="1"/>
-    <col min="5" max="5" width="13.41796875" customWidth="1"/>
-    <col min="8" max="8" width="10.26171875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.15625" customWidth="1"/>
+    <col min="3" max="3" width="14.68359375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="10.5234375" customWidth="1"/>
+    <col min="5" max="5" width="12.05078125" customWidth="1"/>
+    <col min="6" max="6" width="13.41796875" customWidth="1"/>
+    <col min="9" max="9" width="10.26171875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="1" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:10" s="1" customFormat="1" ht="17.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5"/>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
-    </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J1" s="5"/>
+    </row>
+    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="15">
+        <v>45293</v>
+      </c>
+      <c r="C2" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="5">
+      <c r="D2" s="5">
         <v>5</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="7">
         <v>220</v>
       </c>
-      <c r="E2" s="7">
-        <f>C2*D2</f>
+      <c r="F2" s="7">
+        <f>D2*E2</f>
         <v>1100</v>
       </c>
-      <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6"/>
       <c r="I2" s="6"/>
-    </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J2" s="6"/>
+    </row>
+    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="15">
+        <v>45293</v>
+      </c>
+      <c r="C3" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5">
+      <c r="D3" s="5">
         <v>7</v>
       </c>
-      <c r="D3" s="7">
+      <c r="E3" s="7">
         <v>575</v>
       </c>
-      <c r="E3" s="7">
-        <f t="shared" ref="E3:E14" si="0">C3*D3</f>
+      <c r="F3" s="7">
+        <f t="shared" ref="F3:F14" si="0">D3*E3</f>
         <v>4025</v>
       </c>
-      <c r="F3" s="6"/>
       <c r="G3" s="6"/>
       <c r="H3" s="6"/>
       <c r="I3" s="6"/>
-    </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="15">
+        <v>45366</v>
+      </c>
+      <c r="C4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C4" s="5">
+      <c r="D4" s="5">
         <v>6</v>
       </c>
-      <c r="D4" s="7">
+      <c r="E4" s="7">
         <v>139</v>
       </c>
-      <c r="E4" s="7">
+      <c r="F4" s="7">
         <f t="shared" si="0"/>
         <v>834</v>
       </c>
-      <c r="F4" s="6"/>
       <c r="G4" s="6"/>
       <c r="H4" s="6"/>
       <c r="I4" s="6"/>
-    </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J4" s="6"/>
+    </row>
+    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="15">
+        <v>45366</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="5">
+      <c r="D5" s="5">
         <v>8</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>117.75</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
         <v>942</v>
       </c>
-      <c r="F5" s="6"/>
       <c r="G5" s="6"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J5" s="6"/>
+    </row>
+    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B6" s="12" t="s">
+      <c r="B6" s="15">
+        <v>45450</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="5">
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>575</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="7">
         <f t="shared" si="0"/>
         <v>2300</v>
       </c>
-      <c r="F6" s="6"/>
       <c r="G6" s="6"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
-    </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12" t="s">
+      <c r="B7" s="15">
+        <v>45450</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="5">
+      <c r="D7" s="5">
         <v>10</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>459</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <f t="shared" si="0"/>
         <v>4590</v>
       </c>
-      <c r="F7" s="6"/>
       <c r="G7" s="6"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
-    </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J7" s="6"/>
+    </row>
+    <row r="8" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="15">
+        <v>45450</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="5">
+      <c r="D8" s="5">
         <v>12</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>199.99</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <f t="shared" si="0"/>
         <v>2399.88</v>
       </c>
-      <c r="F8" s="6"/>
       <c r="G8" s="6"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
-    </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J8" s="6"/>
+    </row>
+    <row r="9" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="15">
+        <v>45343</v>
+      </c>
+      <c r="C9" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="5">
+      <c r="D9" s="5">
         <v>8</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="7">
         <v>384.45</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <f t="shared" si="0"/>
         <v>3075.6</v>
       </c>
-      <c r="F9" s="6"/>
       <c r="G9" s="6"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
-    </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J9" s="6"/>
+    </row>
+    <row r="10" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="15">
+        <v>45398</v>
+      </c>
+      <c r="C10" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="C10" s="5">
+      <c r="D10" s="5">
         <v>-4</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="7">
         <v>245</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <f t="shared" si="0"/>
         <v>-980</v>
       </c>
-      <c r="F10" s="6"/>
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
-    </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J10" s="6"/>
+    </row>
+    <row r="11" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="15">
+        <v>45398</v>
+      </c>
+      <c r="C11" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="5">
+      <c r="D11" s="5">
         <v>-5</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="7">
         <v>660</v>
       </c>
-      <c r="E11" s="7">
+      <c r="F11" s="7">
         <f t="shared" si="0"/>
         <v>-3300</v>
       </c>
-      <c r="F11" s="6"/>
       <c r="G11" s="6"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
-    </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J11" s="6"/>
+    </row>
+    <row r="12" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="15">
+        <v>45595</v>
+      </c>
+      <c r="C12" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C12" s="5">
+      <c r="D12" s="5">
         <v>8</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="7">
         <v>443</v>
       </c>
-      <c r="E12" s="7">
+      <c r="F12" s="7">
         <f t="shared" si="0"/>
         <v>3544</v>
       </c>
-      <c r="F12" s="6"/>
       <c r="G12" s="6"/>
       <c r="H12" s="6"/>
       <c r="I12" s="6"/>
-    </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J12" s="6"/>
+    </row>
+    <row r="13" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="12" t="s">
+      <c r="B13" s="15">
+        <v>45595</v>
+      </c>
+      <c r="C13" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="5">
+      <c r="D13" s="5">
         <v>15</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E13" s="7">
         <v>224.9</v>
       </c>
-      <c r="E13" s="7">
+      <c r="F13" s="7">
         <f t="shared" si="0"/>
         <v>3373.5</v>
       </c>
-      <c r="F13" s="6"/>
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="6"/>
-    </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J13" s="6"/>
+    </row>
+    <row r="14" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="15">
+        <v>45492</v>
+      </c>
+      <c r="C14" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5">
+      <c r="D14" s="5">
         <v>-5</v>
       </c>
-      <c r="D14" s="7">
+      <c r="E14" s="7">
         <v>459</v>
       </c>
-      <c r="E14" s="7">
+      <c r="F14" s="7">
         <f t="shared" si="0"/>
         <v>-2295</v>
       </c>
-      <c r="F14" s="6"/>
       <c r="G14" s="6"/>
       <c r="H14" s="6"/>
       <c r="I14" s="6"/>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J14" s="6"/>
+    </row>
+    <row r="15" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6"/>
-      <c r="B15" s="10"/>
-      <c r="C15" s="6"/>
+      <c r="B15" s="13"/>
+      <c r="C15" s="10"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="6"/>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>
-    </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J15" s="6"/>
+    </row>
+    <row r="16" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6"/>
-      <c r="B16" s="10"/>
-      <c r="C16" s="6"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="10"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
       <c r="G16" s="6"/>
       <c r="H16" s="6"/>
       <c r="I16" s="6"/>
-    </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J16" s="6"/>
+    </row>
+    <row r="17" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6"/>
-      <c r="B17" s="10"/>
-      <c r="C17" s="6"/>
+      <c r="B17" s="13"/>
+      <c r="C17" s="10"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="6"/>
       <c r="H17" s="6"/>
       <c r="I17" s="6"/>
-    </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J17" s="6"/>
+    </row>
+    <row r="18" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6"/>
-      <c r="B18" s="10"/>
-      <c r="C18" s="6"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="10"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="6"/>
       <c r="H18" s="6"/>
       <c r="I18" s="6"/>
-    </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="J18" s="6"/>
+    </row>
+    <row r="19" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6"/>
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
+      <c r="B19" s="13"/>
+      <c r="C19" s="10"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
       <c r="H19" s="6"/>
       <c r="I19" s="6"/>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J19" s="6"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="8"/>
-      <c r="B20" s="11"/>
-      <c r="C20" s="8"/>
+      <c r="B20" s="14"/>
+      <c r="C20" s="11"/>
       <c r="D20" s="8"/>
       <c r="E20" s="8"/>
       <c r="F20" s="8"/>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
       <c r="I20" s="8"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J20" s="8"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="8"/>
-      <c r="B21" s="11"/>
-      <c r="C21" s="8"/>
+      <c r="B21" s="14"/>
+      <c r="C21" s="11"/>
       <c r="D21" s="8"/>
       <c r="E21" s="8"/>
       <c r="F21" s="8"/>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
       <c r="I21" s="8"/>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="J21" s="8"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="8"/>
-      <c r="B22" s="11"/>
-      <c r="C22" s="8"/>
+      <c r="B22" s="14"/>
+      <c r="C22" s="11"/>
       <c r="D22" s="8"/>
       <c r="E22" s="8"/>
       <c r="F22" s="8"/>
       <c r="G22" s="8"/>
       <c r="H22" s="8"/>
       <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>